<commit_message>
wip: switched to master version of excelize because bug
</commit_message>
<xml_diff>
--- a/drivers/xlsx/testdata/test_date2.xlsx
+++ b/drivers/xlsx/testdata/test_date2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilotoole/work/sq/sq/drivers/xlsx/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE8AE85-0EFB-4248-BFB1-C3B73B425635}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF71122-077C-144F-9095-D0D533B26834}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="74760" yWindow="8860" windowWidth="32740" windowHeight="19280" xr2:uid="{CB076863-889C-1B46-B85A-ED78C32E1EED}"/>
   </bookViews>
@@ -25,25 +25,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>when1</t>
+    <t>col_time</t>
+  </si>
+  <si>
+    <t>col_time_n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,9 +76,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,33 +396,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B72B6E-F485-EA40-8BC1-C521818CA470}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>32769</v>
-      </c>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>32763</v>
-      </c>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>0.29660879629955161</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.29660879629955161</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>0.29662037037037037</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>